<commit_message>
add campo degradado no ind 4 + add tabelas ind 2
</commit_message>
<xml_diff>
--- a/indicadores/04/tabelas/2002_bacias.xlsx
+++ b/indicadores/04/tabelas/2002_bacias.xlsx
@@ -12,16 +12,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
-    <t>LEGENDA</t>
+    <t>legenda</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>nome</t>
   </si>
   <si>
     <t>area_km2</t>
-  </si>
-  <si>
-    <t>nome</t>
-  </si>
-  <si>
-    <t>area_km2_1</t>
   </si>
   <si>
     <t>Extensão de agricultura e silvicultura (ano-base 2002)</t>
@@ -179,7 +179,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>7879.37667881</v>
+        <v>13141.9972595</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -193,7 +193,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>889.222071542</v>
+        <v>1638.95622443</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -207,7 +207,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>7094.42920502</v>
+        <v>9254.16171808</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -221,7 +221,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1059.39911774</v>
+        <v>1567.77845243</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -235,7 +235,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1139.23337754</v>
+        <v>2116.88353751</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -249,7 +249,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>2167.1969414</v>
+        <v>3942.25013061</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -263,7 +263,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>3892.22357294</v>
+        <v>7150.98928162</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -277,7 +277,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>4257.72852062</v>
+        <v>6328.53226945</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -291,7 +291,7 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <v>1797.50704122</v>
+        <v>1849.3153882</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -305,7 +305,7 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <v>688.542121057</v>
+        <v>884.441544154</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -319,7 +319,7 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <v>7360.2179521</v>
+        <v>10245.6747183</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
@@ -333,7 +333,7 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <v>2195.4489569</v>
+        <v>2321.51552537</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -347,7 +347,7 @@
         <v>4</v>
       </c>
       <c r="B14">
-        <v>313.749446676</v>
+        <v>328.721732755</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -361,7 +361,7 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>1756.28735316</v>
+        <v>1997.06759274</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -375,7 +375,7 @@
         <v>4</v>
       </c>
       <c r="B16">
-        <v>10280.0269769</v>
+        <v>17473.66252</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
@@ -389,7 +389,7 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <v>2573.15509911</v>
+        <v>4106.52340143</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -403,7 +403,7 @@
         <v>4</v>
       </c>
       <c r="B18">
-        <v>10322.0744421</v>
+        <v>10718.4168586</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
@@ -417,7 +417,7 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <v>4269.41254688</v>
+        <v>5301.42115388</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
@@ -431,7 +431,7 @@
         <v>4</v>
       </c>
       <c r="B20">
-        <v>9617.832294510001</v>
+        <v>9874.269802430001</v>
       </c>
       <c r="C20" t="s">
         <v>23</v>
@@ -445,7 +445,7 @@
         <v>4</v>
       </c>
       <c r="B21">
-        <v>8956.60373875</v>
+        <v>9820.44094998</v>
       </c>
       <c r="C21" t="s">
         <v>24</v>
@@ -459,7 +459,7 @@
         <v>4</v>
       </c>
       <c r="B22">
-        <v>4163.20476159</v>
+        <v>4166.36667473</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
@@ -473,7 +473,7 @@
         <v>4</v>
       </c>
       <c r="B23">
-        <v>9844.902112219999</v>
+        <v>9852.6254023</v>
       </c>
       <c r="C23" t="s">
         <v>26</v>
@@ -487,7 +487,7 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>8445.61597241</v>
+        <v>8445.983877320001</v>
       </c>
       <c r="C24" t="s">
         <v>27</v>
@@ -501,7 +501,7 @@
         <v>4</v>
       </c>
       <c r="B25">
-        <v>955.559428237</v>
+        <v>1337.14824275</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
@@ -515,7 +515,7 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>13724.6001388</v>
+        <v>14911.9201979</v>
       </c>
       <c r="C26" t="s">
         <v>29</v>

</xml_diff>